<commit_message>
FIX: Tracking metrics and saving visualizations to show in metrics and image section of each job
</commit_message>
<xml_diff>
--- a/results/transcript/I Built a Self Landing Satellite.xlsx
+++ b/results/transcript/I Built a Self Landing Satellite.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C183"/>
+  <dimension ref="A1:C131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,7 +453,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>This is a satellite that turns into a drone.</t>
+          <t>This is a satellite that turns into a drone, and today we're going to be launching a kilometer into the sky, just like that.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -463,3084 +463,2200 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>00:00:02</t>
+          <t>00:00:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>And today we're going to be launching a kilometer into the sky just like that.</t>
+          <t>You're probably a bit confused right now, so let me explain. Basically there's a spleen called a cansaic,</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>00:00:02</t>
+          <t>00:00:11</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>00:00:08</t>
+          <t>00:00:17</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>You're probably a bit confused right now, so let me explain.</t>
+          <t>which is a cansaic satellite that gets launched in a rocket and performs some sort of scientific mission on the way down.</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>00:00:12</t>
+          <t>00:00:17</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>00:00:15</t>
+          <t>00:00:23</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Basically, there's this thing called a Cansat, which is a Kansai satellite that gets launched in a rocket and performs some sort of scientific mission on the way down.</t>
+          <t>Now usually the descent is done with a parachute, but parachutes are kind of lame,</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>00:00:15</t>
+          <t>00:00:24</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>00:00:23</t>
+          <t>00:00:27</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Now, usually the descent is done with a parachute, but parachute parachutes are kind of lame.</t>
+          <t>so what if we generated our own thrust and good guided landing?</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>00:00:24</t>
+          <t>00:00:27</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>00:00:28</t>
+          <t>00:00:32</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>So what if we generated our own thrust and did guided landing?</t>
+          <t>These are some of the smallest propellers I could find at only two inches, and these are way to</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>00:00:28</t>
+          <t>00:00:38</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>00:00:32</t>
+          <t>00:00:45</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>These are some of the smallest propellers I could find at only 2 inches.</t>
+          <t>second. Okay, so I did not order this. I think they gave me the rod pack. I guess we're using this</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>00:00:39</t>
+          <t>00:00:45</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>00:00:43</t>
+          <t>00:00:51</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>And these are.</t>
+          <t>motor then. As you might already tell, the plan is to use propellers to control the descent,</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>00:00:43</t>
+          <t>00:00:51</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>00:00:44</t>
+          <t>00:00:56</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Wait a second.</t>
+          <t>and using this mechanism allows them to fold inward so that it's compact enough to fit in the rocket.</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>00:00:44</t>
+          <t>00:00:56</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>00:00:45</t>
+          <t>00:01:02</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Okay, so I did not order this.</t>
+          <t>Many people have actually tried similar controlled descent missions in the past,</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>00:00:46</t>
+          <t>00:01:02</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>00:00:48</t>
+          <t>00:01:05</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>I think they gave me the Ron pack.</t>
+          <t>but it seems like no one has done so successfully, so maybe we'll be the first.</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>00:00:48</t>
+          <t>00:01:05</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>00:00:49</t>
+          <t>00:01:10</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>I guess we're using this motor then.</t>
+          <t>These motors are super cute, but unfortunately the wires are too short, so let's solder on some longer ones.</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>00:00:50</t>
+          <t>00:01:10</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>00:00:52</t>
+          <t>00:01:16</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>As you might already tell, the plan is to use propellers to control the descent.</t>
+          <t>Now that we have our four motors, we just need a way to lock and release the arms.</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>00:00:53</t>
+          <t>00:01:27</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>00:00:56</t>
+          <t>00:01:32</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>And using this mechanism allows them to fold inward so that it's compact enough to fit in the rocket.</t>
+          <t>Now there are three main ways of doing this. We can have a plate that turns,</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>00:00:56</t>
+          <t>00:01:32</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>00:01:02</t>
+          <t>00:01:36</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Many people have actually tried similar controlled descent missions in the past, but it seems like no one has done so successfully, so maybe we'll be the first.</t>
+          <t>we can have a plate that moves vertically, or we can have a wire that gets cut or burned.</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>00:01:02</t>
+          <t>00:01:36</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>00:01:10</t>
+          <t>00:01:41</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>These motors are super cute, but unfortunately, the wires are too short, so let's solder on some longer ones.</t>
+          <t>The obvious choice is to plate that moves vertically, as the rotating one is more complex,</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>00:01:10</t>
+          <t>00:01:41</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>00:01:16</t>
+          <t>00:01:45</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Now that we have our four motors, we just need a way to lock and release the arms.</t>
+          <t>and cutting the wires both unreliable and hard to reset. However, the servo motors I plan to use</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>00:01:28</t>
+          <t>00:01:45</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>00:01:32</t>
+          <t>00:01:50</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Now, there are three main ways of doing this.</t>
+          <t>rotates, so maybe the rotating method makes more sense, but they're also pretty huge,</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>00:01:32</t>
+          <t>00:01:50</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>00:01:34</t>
+          <t>00:01:55</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>We can have a plate that turns, we can have a plate that moves vertically, or we can have a wire that gets cut or burned.</t>
+          <t>so is there an alternative? Then out of nowhere, I discovered the best invention in human history.</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>00:01:35</t>
+          <t>00:01:55</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>00:01:41</t>
+          <t>00:02:00</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>The obvious choice is the plate that moves vertically, as the rotating one is more complex and cutting the wire is both unreliable and hard to reset.</t>
+          <t>Nope, it's not fire, it's not the internet, and it's not that plane over there.</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>00:01:41</t>
+          <t>00:02:00</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>00:01:48</t>
+          <t>00:02:05</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>However, the servo motors plan to use rotates, so maybe the rotating method makes more sense, but they're also pretty huge.</t>
+          <t>It's this, a 1.5G linear servo motor. It's absolutely tiny, and best of all, it uses a warm gear</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>00:01:48</t>
+          <t>00:02:07</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>00:01:55</t>
+          <t>00:02:15</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>So is there an alternative?</t>
+          <t>to move linearly rather than... So let's make a quick mechanism for it, and...</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>00:01:55</t>
+          <t>00:02:15</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>00:01:56</t>
+          <t>00:02:21</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Then, out of nowhere, I discovered the best invention in human history.</t>
+          <t>It seems like because of the long lever arm here, the release mechanism gets stuck due to friction,</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>00:01:56</t>
+          <t>00:02:22</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>00:02:00</t>
+          <t>00:02:27</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Nope, it's not fire, it's not the Internet, and it's not that plane over there.</t>
+          <t>so I modeled this new one with space for two servo motors. In doing so, I also discovered that</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>00:02:00</t>
+          <t>00:02:28</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>00:02:05</t>
+          <t>00:02:33</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>It's this, a 1.5G linear servo motor.</t>
+          <t>pushing against a flat surface creates much less friction than pushing against a corner.</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>00:02:06</t>
+          <t>00:02:33</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>00:02:12</t>
+          <t>00:02:37</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>It's absolutely tiny.</t>
+          <t>It's really small things like this that make mechanical engineering just so fascinating.</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>00:02:12</t>
+          <t>00:02:38</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>00:02:13</t>
+          <t>00:02:42</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>And best of all, it uses a warm gear to move linearly rather than.</t>
+          <t>After modeling a more finalized upper section, I think it's time for our first proper prototype.</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>00:02:13</t>
+          <t>00:02:44</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>00:02:17</t>
+          <t>00:02:50</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>So let's make a quick mechanism for it.</t>
+          <t>This is probably one of my best CAD designs by far. Every single part is made with intention,</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>00:02:18</t>
+          <t>00:02:50</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>00:02:20</t>
+          <t>00:02:55</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>And it seems like because of the lawn lever arm here, the release mechanism gets stuck due to friction.</t>
+          <t>everything is held together with screws rather than super glue. It's intricate, but easy to print,</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>00:02:20</t>
+          <t>00:02:55</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>00:02:27</t>
+          <t>00:03:00</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>So I modeled this new one with space for two servo motors.</t>
+          <t>it's just so beautiful.</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>00:02:27</t>
+          <t>00:03:00</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>00:02:31</t>
+          <t>00:03:02</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>In doing so, I also discovered that pushing against a flat surface creates much less friction than pushing against a corner.</t>
+          <t>Okay, so here's the release mechanism, here are the middle plates, and here's the top section.</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>00:02:31</t>
+          <t>00:03:24</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>00:02:38</t>
+          <t>00:03:28</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>It's really small things like this that make mechanical engineering just so fascinating.</t>
+          <t>The four arms need a bit of sanding, and after that they can be screwed into place.</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>00:02:38</t>
+          <t>00:03:28</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>00:02:43</t>
+          <t>00:03:32</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>After modeling a more finalized upper section, I think it's time for our first proper prototype.</t>
+          <t>At this point, I realized that the arms were slightly misaligned, so I printed some new ones,</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>00:02:45</t>
+          <t>00:03:38</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>00:02:50</t>
+          <t>00:03:42</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>This is probably one of my Best CAD designs by far.</t>
+          <t>but turns out I printed the Ron file, and they were still misaligned, so I printed it again, and they were STUP!</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>00:02:50</t>
+          <t>00:03:42</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>00:02:53</t>
+          <t>00:03:47</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Every single part is made with intention.</t>
+          <t>And now they are finally perfect.</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>00:02:53</t>
+          <t>00:03:56</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>00:02:55</t>
+          <t>00:03:59</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Everything is held together with screws rather than super glue.</t>
+          <t>We can screw on our servo motors, and...</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>00:02:55</t>
+          <t>00:04:00</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>00:02:58</t>
+          <t>00:04:02</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>It's intricate, but easy to print.</t>
+          <t>Nice!</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>00:02:58</t>
+          <t>00:04:04</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>00:03:00</t>
+          <t>00:04:04</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>It's just so beautiful.</t>
+          <t>Let's move on to electronics. We need a video transmitter to record and transmit video,</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>00:03:00</t>
+          <t>00:04:06</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>00:03:02</t>
+          <t>00:04:11</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Okay, so here's the release mechanism, here are the middle plates, and here's the top section.</t>
+          <t>a fly controller to keep the drone stabilized, and ESC to control the speed of the motors,</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>00:03:24</t>
+          <t>00:04:11</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>00:03:28</t>
+          <t>00:04:15</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>The forearms need a bit of sanding, and after that they can be screwed into place.</t>
+          <t>and in Arduino Nano to transmit scientific data back to the ground from our onboard sensors.</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>00:03:28</t>
+          <t>00:04:15</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>00:03:32</t>
+          <t>00:04:20</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>At this point, I realized that the arms were slightly misaligned, so I printed some new ones.</t>
+          <t>Two of my friends are actually already working on that part, so I'm going to focus on these ones.</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>00:03:38</t>
+          <t>00:04:20</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>00:03:42</t>
+          <t>00:04:25</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>But turns out I printed the wrong file and they were still misaligned.</t>
+          <t>The fly controller and ESC I have here are a bit too big, so I found this smaller one that</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>00:03:42</t>
+          <t>00:04:25</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>00:03:45</t>
+          <t>00:04:29</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>So I printed it again and they were st.</t>
+          <t>combines both into the same board, because this board is just so small, it was pretty challenging</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>00:03:45</t>
+          <t>00:04:29</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>00:03:47</t>
+          <t>00:04:34</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>And now they are finally perfect.</t>
+          <t>to solder. In fact, I broke one of the pads, which genuinely scared me so much, but luckily there</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>00:03:57</t>
+          <t>00:04:34</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>00:03:59</t>
+          <t>00:04:39</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>We can screw on our servo motors and.</t>
+          <t>was an identical pad on the other side. To program the drone, the original intention was to use</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>00:04:00</t>
+          <t>00:04:39</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>00:04:03</t>
+          <t>00:04:44</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Nice.</t>
+          <t>a software called Ardupilot, so we could reform a fully autonomous GPS guided landing.</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>00:04:04</t>
+          <t>00:04:44</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>00:04:04</t>
+          <t>00:04:49</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Let's move on to electronics.</t>
+          <t>But turns out, putting a GPS guided system that targets a specific ground location on a rocket</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>00:04:06</t>
+          <t>00:04:50</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>00:04:08</t>
+          <t>00:04:54</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>We need a video transmitter to record and transmit video.</t>
+          <t>traveling 200 plus miles per hour might not be the best idea. We also couldn't get a</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>00:04:08</t>
+          <t>00:04:54</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>00:04:10</t>
+          <t>00:04:59</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>A flight controller to keep the drone stabilized, an ESC to control the speed of the motors, and an Arduino Nano to transmit scientific data back to the ground from our onboard sensors.</t>
+          <t>compatible flight controller in time, so we are forced to manually control the cance from the</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>00:04:10</t>
+          <t>00:04:59</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>00:04:20</t>
+          <t>00:05:04</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Two of my friends are actually already working on that part, so I'm going to focus on these ones.</t>
+          <t>ground using a software called BataFlight, which is meant for FPV drones, but whatever.</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>00:04:20</t>
+          <t>00:05:04</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>00:04:25</t>
+          <t>00:05:09</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>The flight controller and ESC I have here are a bit too big, so I found this smaller one that combines both into the same board.</t>
+          <t>Here I am setting some basic settings that are needed for the drone to fly. The controller has</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>00:04:25</t>
+          <t>00:05:09</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>00:04:31</t>
+          <t>00:05:13</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Because this board is just so small, it was pretty challenging to.</t>
+          <t>to be set up to communicate, and we need an arm switch, which is basically a safety switch</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>00:04:31</t>
+          <t>00:05:13</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>00:04:35</t>
+          <t>00:05:17</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>In fact, I broke one of the pads, which genuinely scared me so much.</t>
+          <t>to unlock the drone when you're ready to fly. There's also a safety feature that prevents the</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>00:04:35</t>
+          <t>00:05:17</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>00:04:39</t>
+          <t>00:05:22</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>But luckily there was an identical pad on the other side to program the drone.</t>
+          <t>drone from arming when it's moving too quickly, or sitting at an angle. But we need a bypass</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>00:04:39</t>
+          <t>00:05:22</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>00:04:43</t>
+          <t>00:05:26</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>The original intention was to use a software called Ardupilot so we could perform a fully autonomous GPS guided landing.</t>
+          <t>it so we can arm the drone even when it's tumbling violently as it exits the rocket, like this.</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>00:04:43</t>
+          <t>00:05:26</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>00:04:49</t>
+          <t>00:05:32</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>But turns out putting a GPS guided system that targets a specific ground location on a rocket traveling 200 miles per hour might not be the best idea.</t>
+          <t>Other my calculations say that the motor's providing a thrust, I still kind of doubt that these</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>00:04:49</t>
+          <t>00:05:35</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>00:04:58</t>
+          <t>00:05:40</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>We also couldn't get a compatible flight controller in time, so we are forced to manually control the Cansat from the ground using a software code called BetaFlight, which is meant for FPV drones, but whatever.</t>
+          <t>tiny propellers are all that's needed to make this thing fly. So if this doesn't work, this project</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>00:04:58</t>
+          <t>00:05:40</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>00:05:09</t>
+          <t>00:05:46</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Here I am setting some basic settings that are needed for the drone to fly.</t>
+          <t>might be screwed.</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>00:05:09</t>
+          <t>00:05:46</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>00:05:12</t>
+          <t>00:05:47</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>The controller has to be set up to communicate, and we need an arm switch, which is basically a safety switch to unlock the drone when you're ready to fly.</t>
+          <t>We're still far from finished, however, there are a lot of tiny things we need to change.</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>00:05:12</t>
+          <t>00:06:07</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>00:05:20</t>
+          <t>00:06:12</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>There's also a safety feature that prevents the drone from arming when it's moving too quickly or sitting at an angle.</t>
+          <t>For example, it was only after I added the motors that I realized these screws</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>00:05:20</t>
+          <t>00:06:12</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>00:05:25</t>
+          <t>00:06:15</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>But we need to bypass it so we can arm the drone even when it's tumbling violently as it exits the the rocket like this.</t>
+          <t>were up against the walls and caused too much friction for the arms to open, so we need to make</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>00:05:25</t>
+          <t>00:06:15</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>00:05:32</t>
+          <t>00:06:20</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Although my calculations say that the motors provide enough thrust, I still kind of doubt that these tiny propellers are all that's needed to make this thing fly.</t>
+          <t>some room for that. We also need to make some room for a plug here, we also need to make some room</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>00:05:35</t>
+          <t>00:06:20</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>00:05:44</t>
+          <t>00:06:24</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>So if this doesn't work, this project might be Screwed.</t>
+          <t>for this capacitor, we also need to make some room for the wires that go down, we need room for</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>00:05:44</t>
+          <t>00:06:24</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>00:05:47</t>
+          <t>00:06:28</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Yo, yo, yo, guys.</t>
+          <t>the camera cable that goes down. Oh yeah, we need room for this fan on the top because the video</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>00:06:00</t>
+          <t>00:06:28</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>00:06:02</t>
+          <t>00:06:32</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>That is actually so cool.</t>
+          <t>transmitter tends to overheat. Speaking of the fan while I was soldering it on, I kind of messed up.</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>00:06:05</t>
+          <t>00:06:32</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>00:06:06</t>
+          <t>00:06:39</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>We're still far from finished.</t>
+          <t>So for some reason, when I tried to plug the board in after soldering on the fan, there was a short</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>00:06:08</t>
+          <t>00:06:40</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>00:06:09</t>
+          <t>00:06:44</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>However, there are a lot of tiny things we need to change.</t>
+          <t>board and thank god I had the short stopper on because if I did it, this project would have</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>00:06:09</t>
+          <t>00:06:44</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>00:06:12</t>
+          <t>00:06:48</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>For example, it was only after I added the motors that I realized these screws rub against the walls and caused too much friction for the arms to open.</t>
+          <t>actually just been over. Then I realized this small blob of solder was probably the issue,</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>00:06:12</t>
+          <t>00:06:48</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>00:06:19</t>
+          <t>00:06:52</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>So we need to make some room for that.</t>
+          <t>so when I remove it, it was finally fixed. Fan spins as well. Look at that, that is perfect.</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>00:06:19</t>
+          <t>00:06:52</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>00:06:20</t>
+          <t>00:07:03</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>We also need to make some room for a plug here.</t>
+          <t>Cramping all these electronics into the tiny can genuinely took so long due to many</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>00:06:20</t>
+          <t>00:07:09</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>00:06:23</t>
+          <t>00:07:14</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>We also need to make some room for this capacitor.</t>
+          <t>unforeseen issues. Like for example, the video transmitter didn't have holes on the bottom,</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>00:06:23</t>
+          <t>00:07:14</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>00:06:25</t>
+          <t>00:07:19</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>We also need to make some room for the wires that go down.</t>
+          <t>so I had to force in these tiny nuts to hold it in place.</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>00:06:25</t>
+          <t>00:07:19</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>00:06:28</t>
+          <t>00:07:21</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>We need for the camera cable that goes down.</t>
+          <t>These screws are kind of funny because if you try to use force it ends up falling out or</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>00:06:28</t>
+          <t>00:07:33</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>00:06:30</t>
+          <t>00:07:37</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Oh, yeah, we need room for this fan on the top because the video transmitter tends to overheat.</t>
+          <t>getting misaligned, but if you stay calm, you're much more likely to succeed first try,</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>00:06:30</t>
+          <t>00:07:37</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>00:06:34</t>
+          <t>00:07:42</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Speaking of the fan, while I was soldering it on, I kind of messed up.</t>
+          <t>which I guess is kind of an analogy for other things in life as well.</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>00:06:35</t>
+          <t>00:07:42</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>00:06:40</t>
+          <t>00:07:46</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>So for some reason, when I tried to plug the board in after soldering on the fan, there was a short.</t>
+          <t>Putting in all these screws is kind of annoying, but I'm just so glad that there's no super</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>00:06:40</t>
+          <t>00:07:49</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>00:06:44</t>
+          <t>00:07:53</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>And thank God I had the short stopper on, because if I didn't, this project would have actually just been over.</t>
+          <t>glue or tuck tape. Now we can just attach all four of the arms and screw on the motors one by one</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>00:06:44</t>
+          <t>00:07:53</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>00:06:49</t>
+          <t>00:07:59</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Then I realized this small blob of solder was probably the issue.</t>
+          <t>in the super cool time lapse. And just like that, the densely filled upper section is done,</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>00:06:49</t>
+          <t>00:07:59</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>00:06:52</t>
+          <t>00:08:04</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>So when I removed it.</t>
+          <t>and of course the arms release perfectly. I also printed the centenum mount out of TPU,</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>00:06:52</t>
+          <t>00:08:04</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>00:06:53</t>
+          <t>00:08:09</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Yes.</t>
+          <t>which fits snugly and secures onto the top of the can. The bottom section is a lot more simple</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>00:06:55</t>
+          <t>00:08:09</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>00:06:55</t>
+          <t>00:08:14</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Let's go, let's go.</t>
+          <t>and printed in one piece. The bottom holds the FBV camera, the battery of the sliding door to</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>00:06:55</t>
+          <t>00:08:14</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>00:06:57</t>
+          <t>00:08:23</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>It was finally fixed.</t>
+          <t>lock in place, the receiver for my transmitter, and the Arduino Nano, which is hooked up to some</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>00:06:57</t>
+          <t>00:08:23</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>00:06:59</t>
+          <t>00:08:29</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Fan spins as well.</t>
+          <t>sensors and a radio to send real time data like altitude and temperature back to the ground station.</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>00:07:00</t>
+          <t>00:08:29</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>00:07:01</t>
+          <t>00:08:33</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Look at that.</t>
+          <t>Speaking of that, my friends working on the Arduino spent like three days on it but couldn't</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>00:07:01</t>
+          <t>00:08:34</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>00:07:02</t>
+          <t>00:08:38</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>That is perfect.</t>
+          <t>get it to work so I tried to help, but I think I just made it worse.</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>00:07:02</t>
+          <t>00:08:38</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>00:07:03</t>
+          <t>00:08:41</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Cramming all these electronics into the tiny can genuinely took so long due to many unforeseen issues, like, for example, the video transmitter didn't have holes on the bottom, so I had to force in these tiny nuts to hold it in place.</t>
+          <t>Turns out literally half the components we were using were somehow damaged, so one of my friends</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>00:07:09</t>
+          <t>00:08:59</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>00:07:21</t>
+          <t>00:09:04</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>These screws are kind of funny because if you try to use force, it ends up falling out or getting misaligned.</t>
+          <t>volunteered to drive all the way down to the US so that he could buy parts in time before the</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>00:07:33</t>
+          <t>00:09:04</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>00:07:38</t>
+          <t>00:09:09</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>But if you stay calm, you're much more likely to succeed first try.</t>
+          <t>launch, and then I kid you not on a day before we had to fly out it finally worked.</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>00:07:38</t>
+          <t>00:09:09</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>00:07:42</t>
+          <t>00:09:14</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Which I guess is kind of an analogy for other things in life as well.</t>
+          <t>So now let's just secure these components into the lower section,</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>00:07:42</t>
+          <t>00:09:17</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>00:07:46</t>
+          <t>00:09:20</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Putting in all these screws is kind of annoying, but I'm just so glad that there's no super glue or duct tape.</t>
+          <t>join everything with lead screws, and just like that our satellite is finally finished.</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>00:07:49</t>
+          <t>00:09:21</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>00:07:54</t>
+          <t>00:09:26</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Now we can just attach all four of the arms and screw on the motors one by one in this super cool timelapse.</t>
+          <t>I'm a little bit concerned about the strength of these arms, but luckily this video is sponsored</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>00:07:54</t>
+          <t>00:09:26</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>00:08:01</t>
+          <t>00:09:31</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>And just like that, the densely filled upper section is done.</t>
+          <t>by PCBWay. PCBWay offers the best custom PCB prototyping services, but they also offer</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>00:08:01</t>
+          <t>00:09:31</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>00:08:04</t>
+          <t>00:09:37</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>And of course, the arms release perfectly.</t>
+          <t>3D printing, including metal 3D printing. They're subloader files for an instant quote, and PCBWay will</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>00:08:04</t>
+          <t>00:09:37</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>00:08:06</t>
+          <t>00:09:43</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>I also printed this antenna mount out of tpu, which fits snugly and secures onto the top of the can.</t>
+          <t>make and ship the parts directly to your house, and now we have backup aluminum arms that look</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>00:08:06</t>
+          <t>00:09:43</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>00:08:12</t>
+          <t>00:09:48</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>The bottom section is a lot more simple and printed in one piece.</t>
+          <t>absolutely amazing. If you're working on a project and need metal 3D printing or any of these</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>00:08:12</t>
+          <t>00:09:49</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>00:08:15</t>
+          <t>00:09:53</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>The bottom holds the FPV camera, the battery with the sliding door to lock it in place, the receiver for my transmitter, and the Arduino Nano, which is hooked up to some sensors and a radio to send real time data like altitude and temperature back to the ground station.</t>
+          <t>other services, make sure to check them out. I spent the last bit of time troubleshooting some</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>00:08:20</t>
+          <t>00:09:53</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>00:08:34</t>
+          <t>00:09:58</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Speaking of that, my friends working on The Arduino spent like three days on it, but couldn't get it to work.</t>
+          <t>stupid technical stuff, which you can pause here if you are interested, and yeah, let's go launch this thing.</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>00:08:34</t>
+          <t>00:09:58</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>00:08:39</t>
+          <t>00:10:05</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>So I tried to help, but I think I just made it worse.</t>
+          <t>After a 1.5 hour flight, a 2 hour bus ride, and another 1 hour bus ride, we're now in the middle of,</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>00:08:39</t>
+          <t>00:10:25</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>00:08:41</t>
+          <t>00:10:32</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>No.</t>
+          <t>nowhere.</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>00:08:41</t>
+          <t>00:10:37</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>00:08:42</t>
+          <t>00:10:38</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Stupid fuck.</t>
+          <t>We started off the day by watching this other guys rocket launch, which was pretty cool.</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>00:08:45</t>
+          <t>00:10:48</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>00:08:46</t>
+          <t>00:10:53</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Does it wait maybe wait 30 seconds?</t>
+          <t>But immediately afterwards, as we started preparing for our launch, the tension set in.</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>00:08:46</t>
+          <t>00:10:57</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>00:08:48</t>
+          <t>00:11:02</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Because for.</t>
+          <t>Despite our beautiful design, almost no one had confidence in us. After all, guided landing</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>00:08:49</t>
+          <t>00:11:03</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>00:08:49</t>
+          <t>00:11:07</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>For my really simple code, it had to wait like 30 seconds.</t>
+          <t>had been tried so many times, and it seems like all of them fail. There's just way too much</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>00:08:49</t>
+          <t>00:11:07</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>00:08:52</t>
+          <t>00:11:12</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>And it worked.</t>
+          <t>uncertainty when it comes to launching something in a rocket. What if the rotation is too much for</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>00:08:52</t>
+          <t>00:11:12</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>00:08:53</t>
+          <t>00:11:17</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Then start printing error message after 30 seconds.</t>
+          <t>the flight controller to handle? What if this year force of ejection tears the satellite apart?</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>00:08:53</t>
+          <t>00:11:17</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>00:08:58</t>
+          <t>00:11:22</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Turns out literally half the components we were using were somehow damaged.</t>
+          <t>What if we lose connection? To make matters worse, the Arduino Nano that was working just</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>00:09:00</t>
+          <t>00:11:22</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>00:09:03</t>
+          <t>00:11:26</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>So one of my friends volunteered to drive all the way down to the US so that he could buy parts in time before the launch.</t>
+          <t>the previous night randomly refused to send data. But our saddle I was out already being put inside</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>00:09:03</t>
+          <t>00:11:26</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>00:09:09</t>
+          <t>00:11:31</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>And then, I kid you not, on the day before, we had to fly out.</t>
+          <t>the rocket. There was nothing we could do but hope.</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>00:09:09</t>
+          <t>00:11:31</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>00:09:12</t>
+          <t>00:11:34</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>It finally worked.</t>
+          <t>And then, in a turn of events, our launch was delayed, because some other guy was launching a</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>00:09:12</t>
+          <t>00:11:49</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>00:09:14</t>
+          <t>00:11:54</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Yo, let's go, Zach.</t>
+          <t>super large rocket that had priority. And don't get me wrong, his launch was absolutely spectacular.</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>00:09:14</t>
+          <t>00:11:54</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>00:09:16</t>
+          <t>00:12:01</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>So now let's just secure these components into the lower section, join everything with lead screws.</t>
+          <t>But by now, our saddle I had been sitting inside an enclosed rocket for an entire hour,</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>00:09:17</t>
+          <t>00:12:06</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>00:09:23</t>
+          <t>00:12:12</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>And just like that, our satellite is finally finished.</t>
+          <t>and the video transmitter was starting to overheat.</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>00:09:23</t>
+          <t>00:12:12</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>00:09:26</t>
+          <t>00:12:14</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>I'm a little bit concerned about the strength of these arms, but luckily this video is sponsored by PCBway.</t>
+          <t>But right before our launch, miraculously, the fan had somehow managed to call the video transmitter</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>00:09:26</t>
+          <t>00:12:23</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>00:09:32</t>
+          <t>00:12:29</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>PCBway offers the best custom PCB prototyping services, but they also offer 3D printing, including metal 3D printing.</t>
+          <t>down again, and it seemed like maybe, just maybe, everything would be all right.</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>00:09:32</t>
+          <t>00:12:29</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>00:09:40</t>
+          <t>00:12:35</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Just upload your files for an instant quote and pcbway will make and ship the parts directly to your house.</t>
+          <t>We had a pretty rough landing due to of all things pilot error. The plan was to free fall until</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>00:09:40</t>
+          <t>00:13:48</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>00:09:45</t>
+          <t>00:13:54</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>And now we have backup aluminum arms that look absolutely amazing.</t>
+          <t>right about 200 meters above the ground, max out the thrust, and fly back towards the launch site.</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>00:09:45</t>
+          <t>00:13:54</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>00:09:50</t>
+          <t>00:13:59</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>If you're working on a project and need metal 3D printing or any of these other services, make sure to check them out.</t>
+          <t>But due to the stress, and because the landscape looked all the same, I didn't realize that the</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>00:09:50</t>
+          <t>00:13:59</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>00:09:56</t>
+          <t>00:14:03</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>I spent the last bit of time troubleshooting some stupid technical stuff, which you can pause here if you are interested.</t>
+          <t>ground was coming until way too late. Luckily, we knew the general location of the Kansai thanks to</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>00:09:56</t>
+          <t>00:14:03</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>00:10:01</t>
+          <t>00:14:09</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>And yeah, let's go launch this thing.</t>
+          <t>the onboard footage, and it only took us a mere 3-4 minutes before it was located.</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>00:10:02</t>
+          <t>00:14:09</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>00:10:05</t>
+          <t>00:14:15</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>After a 1.5 hour flight, a 2 hour bus ride, and another 1 hour bus ride, we're now in the middle of nowhere.</t>
+          <t>Somehow, the Kansai was still completely intact, with only slight bending in one of the arms.</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>00:10:25</t>
+          <t>00:14:28</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>00:10:33</t>
+          <t>00:14:33</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>All right, guys, ready?</t>
+          <t>So after getting the arms replaced, the satellite was as good as new.</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>00:10:46</t>
+          <t>00:14:34</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>00:10:48</t>
+          <t>00:14:38</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>We started off the day by watching this other guy's rocket launch, which was pretty cool.</t>
+          <t>We even managed to recover our data thanks to this single GeForce indicator. Just make a</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>00:10:48</t>
+          <t>00:14:38</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>00:10:53</t>
+          <t>00:14:43</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>But immediately afterwards, as we started preparing for our launch, the tension set in.</t>
+          <t>program to grab the value from every frame, grab it over time, and do some integration, and now</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>00:10:58</t>
+          <t>00:14:43</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>00:11:03</t>
+          <t>00:14:49</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Despite our beautiful design, almost no one had confidence in us.</t>
+          <t>you have altitude. We spent the rest of the day just flying this thing around randomly for fun,</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>00:11:03</t>
+          <t>00:14:49</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>00:11:06</t>
+          <t>00:14:54</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>After all, guided landing had been tried so many times, and it seems like all of them fail.</t>
+          <t>and we also did this free fall test, and I think I'm now a much better pilot.</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>00:11:06</t>
+          <t>00:14:54</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>00:11:11</t>
+          <t>00:14:59</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>There's just way too much uncertainty when it comes to launching something in a rocket.</t>
+          <t>Speaking of that, we were actually offered a second launch on a bigger and more powerful rocket</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>00:11:11</t>
+          <t>00:14:59</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>00:11:16</t>
+          <t>00:15:03</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>What if the rotation is too much for the flight controller to handle?</t>
+          <t>in Seattle during the summer, so make sure to let me know in the comments if you are interested.</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>00:11:16</t>
+          <t>00:15:03</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>00:11:19</t>
+          <t>00:15:09</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>What if the sheer force of the ejection tears the satellite apart?</t>
+          <t>And with that being said, special thanks to Zach, Daniel, Emery, Eric, and Cynthia for working</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>00:11:19</t>
+          <t>00:15:12</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>00:11:22</t>
+          <t>00:15:18</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>What if we lose connection?</t>
+          <t>on this project with me. Special thanks to everyone at Kansai who made this experience possible.</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>00:11:22</t>
+          <t>00:15:18</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>00:11:23</t>
+          <t>00:15:23</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>To make matters worse, the Arduino Nano that was working just the previous night randomly refused to send data.</t>
+          <t>And thank you to you for watching. See you next time.</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>00:11:23</t>
+          <t>00:15:23</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>00:11:29</t>
-        </is>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="inlineStr">
-        <is>
-          <t>But our satellite was now already being put inside the rocket.</t>
-        </is>
-      </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>00:11:29</t>
-        </is>
-      </c>
-      <c r="C132" t="inlineStr">
-        <is>
-          <t>00:11:32</t>
-        </is>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="inlineStr">
-        <is>
-          <t>There was nothing we could do but hope.</t>
-        </is>
-      </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>00:11:32</t>
-        </is>
-      </c>
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>00:11:34</t>
-        </is>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="inlineStr">
-        <is>
-          <t>And then, in a turn of events, our launch was delayed because some other guy was launching a super large rocket that had priority.</t>
-        </is>
-      </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>00:11:49</t>
-        </is>
-      </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>00:11:56</t>
-        </is>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>And don't get me wrong, his launch was absolutely spectacular.</t>
-        </is>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>00:11:56</t>
-        </is>
-      </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>00:12:01</t>
-        </is>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="inlineStr">
-        <is>
-          <t>But by now, our satellite had been sitting inside an enclosed rocket for an entire hour, and the video transmitter was starting to overheat.</t>
-        </is>
-      </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>00:12:06</t>
-        </is>
-      </c>
-      <c r="C136" t="inlineStr">
-        <is>
-          <t>00:12:14</t>
-        </is>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" t="inlineStr">
-        <is>
-          <t>It's actually over already.</t>
-        </is>
-      </c>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>00:12:16</t>
-        </is>
-      </c>
-      <c r="C137" t="inlineStr">
-        <is>
-          <t>00:12:17</t>
-        </is>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" t="inlineStr">
-        <is>
-          <t>It doesn't have a chance.</t>
-        </is>
-      </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>00:12:18</t>
-        </is>
-      </c>
-      <c r="C138" t="inlineStr">
-        <is>
-          <t>00:12:20</t>
-        </is>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" t="inlineStr">
-        <is>
-          <t>We can choose not to launch that rocket.</t>
-        </is>
-      </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>00:12:20</t>
-        </is>
-      </c>
-      <c r="C139" t="inlineStr">
-        <is>
-          <t>00:12:22</t>
-        </is>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" t="inlineStr">
-        <is>
-          <t>But right before our launch, miraculously, the fan had somehow managed to cool the video transmitter down again.</t>
-        </is>
-      </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>00:12:23</t>
-        </is>
-      </c>
-      <c r="C140" t="inlineStr">
-        <is>
-          <t>00:12:29</t>
-        </is>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" t="inlineStr">
-        <is>
-          <t>And it seemed maybe, just maybe, everything would be all right.</t>
-        </is>
-      </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>00:12:29</t>
-        </is>
-      </c>
-      <c r="C141" t="inlineStr">
-        <is>
-          <t>00:12:35</t>
-        </is>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" t="inlineStr">
-        <is>
-          <t>We're ready.</t>
-        </is>
-      </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>00:12:37</t>
-        </is>
-      </c>
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>00:12:38</t>
-        </is>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" t="inlineStr">
-        <is>
-          <t>Ready.</t>
-        </is>
-      </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>00:12:38</t>
-        </is>
-      </c>
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>00:12:38</t>
-        </is>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" t="inlineStr">
-        <is>
-          <t>Watching.</t>
-        </is>
-      </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>00:12:38</t>
-        </is>
-      </c>
-      <c r="C144" t="inlineStr">
-        <is>
-          <t>00:12:39</t>
-        </is>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="inlineStr">
-        <is>
-          <t>In five, four, three, two, one.</t>
-        </is>
-      </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>00:12:39</t>
-        </is>
-      </c>
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>00:12:44</t>
-        </is>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="inlineStr">
-        <is>
-          <t>Wait it.</t>
-        </is>
-      </c>
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>00:12:54</t>
-        </is>
-      </c>
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>00:12:56</t>
-        </is>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="inlineStr">
-        <is>
-          <t>Yo.</t>
-        </is>
-      </c>
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>00:13:06</t>
-        </is>
-      </c>
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>00:13:06</t>
-        </is>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>Let's go, let's go, let's go, let's go, let's go, let's go.</t>
-        </is>
-      </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>00:13:06</t>
-        </is>
-      </c>
-      <c r="C148" t="inlineStr">
-        <is>
-          <t>00:13:23</t>
-        </is>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" t="inlineStr">
-        <is>
-          <t>All right, I'm just gonna slow down really fast.</t>
-        </is>
-      </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>00:13:24</t>
-        </is>
-      </c>
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>00:13:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" t="inlineStr">
-        <is>
-          <t>The battery.</t>
-        </is>
-      </c>
-      <c r="B150" t="inlineStr">
-        <is>
-          <t>00:13:26</t>
-        </is>
-      </c>
-      <c r="C150" t="inlineStr">
-        <is>
-          <t>00:13:27</t>
-        </is>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" t="inlineStr">
-        <is>
-          <t>So fast.</t>
-        </is>
-      </c>
-      <c r="B151" t="inlineStr">
-        <is>
-          <t>00:13:27</t>
-        </is>
-      </c>
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>00:13:27</t>
-        </is>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" t="inlineStr">
-        <is>
-          <t>Oh, do you see what I'm seeing, guys?</t>
-        </is>
-      </c>
-      <c r="B152" t="inlineStr">
-        <is>
-          <t>00:13:28</t>
-        </is>
-      </c>
-      <c r="C152" t="inlineStr">
-        <is>
-          <t>00:13:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" t="inlineStr">
-        <is>
-          <t>Okay, wait, wait, wait.</t>
-        </is>
-      </c>
-      <c r="B153" t="inlineStr">
-        <is>
-          <t>00:13:30</t>
-        </is>
-      </c>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>00:13:31</t>
-        </is>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="inlineStr">
-        <is>
-          <t>How many minutes?</t>
-        </is>
-      </c>
-      <c r="B154" t="inlineStr">
-        <is>
-          <t>00:13:31</t>
-        </is>
-      </c>
-      <c r="C154" t="inlineStr">
-        <is>
-          <t>00:13:31</t>
-        </is>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" t="inlineStr">
-        <is>
-          <t>Close to drive.</t>
-        </is>
-      </c>
-      <c r="B155" t="inlineStr">
-        <is>
-          <t>00:13:31</t>
-        </is>
-      </c>
-      <c r="C155" t="inlineStr">
-        <is>
-          <t>00:13:32</t>
-        </is>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" t="inlineStr">
-        <is>
-          <t>Oh, my God.</t>
-        </is>
-      </c>
-      <c r="B156" t="inlineStr">
-        <is>
-          <t>00:13:32</t>
-        </is>
-      </c>
-      <c r="C156" t="inlineStr">
-        <is>
-          <t>00:13:33</t>
-        </is>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" t="inlineStr">
-        <is>
-          <t>Let's go, guys.</t>
-        </is>
-      </c>
-      <c r="B157" t="inlineStr">
-        <is>
-          <t>00:13:33</t>
-        </is>
-      </c>
-      <c r="C157" t="inlineStr">
-        <is>
-          <t>00:13:34</t>
-        </is>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" t="inlineStr">
-        <is>
-          <t>No, I'm scared to go.</t>
-        </is>
-      </c>
-      <c r="B158" t="inlineStr">
-        <is>
-          <t>00:13:35</t>
-        </is>
-      </c>
-      <c r="C158" t="inlineStr">
-        <is>
-          <t>00:13:37</t>
-        </is>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" t="inlineStr">
-        <is>
-          <t>Okay.</t>
-        </is>
-      </c>
-      <c r="B159" t="inlineStr">
-        <is>
-          <t>00:13:37</t>
-        </is>
-      </c>
-      <c r="C159" t="inlineStr">
-        <is>
-          <t>00:13:37</t>
-        </is>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t>I should have flew more.</t>
-        </is>
-      </c>
-      <c r="B160" t="inlineStr">
-        <is>
-          <t>00:13:40</t>
-        </is>
-      </c>
-      <c r="C160" t="inlineStr">
-        <is>
-          <t>00:13:41</t>
-        </is>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="inlineStr">
-        <is>
-          <t>I didn't.</t>
-        </is>
-      </c>
-      <c r="B161" t="inlineStr">
-        <is>
-          <t>00:13:41</t>
-        </is>
-      </c>
-      <c r="C161" t="inlineStr">
-        <is>
-          <t>00:13:42</t>
-        </is>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>I wasn't able to do.</t>
-        </is>
-      </c>
-      <c r="B162" t="inlineStr">
-        <is>
-          <t>00:13:42</t>
-        </is>
-      </c>
-      <c r="C162" t="inlineStr">
-        <is>
-          <t>00:13:43</t>
-        </is>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>Wait, can.</t>
-        </is>
-      </c>
-      <c r="B163" t="inlineStr">
-        <is>
-          <t>00:13:44</t>
-        </is>
-      </c>
-      <c r="C163" t="inlineStr">
-        <is>
-          <t>00:13:45</t>
-        </is>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>Can you fly back?</t>
-        </is>
-      </c>
-      <c r="B164" t="inlineStr">
-        <is>
-          <t>00:13:45</t>
-        </is>
-      </c>
-      <c r="C164" t="inlineStr">
-        <is>
-          <t>00:13:46</t>
-        </is>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>He fly up?</t>
-        </is>
-      </c>
-      <c r="B165" t="inlineStr">
-        <is>
-          <t>00:13:46</t>
-        </is>
-      </c>
-      <c r="C165" t="inlineStr">
-        <is>
-          <t>00:13:47</t>
-        </is>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>No, it's.</t>
-        </is>
-      </c>
-      <c r="B166" t="inlineStr">
-        <is>
-          <t>00:13:47</t>
-        </is>
-      </c>
-      <c r="C166" t="inlineStr">
-        <is>
-          <t>00:13:47</t>
-        </is>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>We had a pretty rough landing due to, of all things, pilot error.</t>
-        </is>
-      </c>
-      <c r="B167" t="inlineStr">
-        <is>
-          <t>00:13:49</t>
-        </is>
-      </c>
-      <c r="C167" t="inlineStr">
-        <is>
-          <t>00:13:52</t>
-        </is>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>The plan was to free fall until right about 200 meters above the ground, max out the thrust, and fly back towards the launch site.</t>
-        </is>
-      </c>
-      <c r="B168" t="inlineStr">
-        <is>
-          <t>00:13:52</t>
-        </is>
-      </c>
-      <c r="C168" t="inlineStr">
-        <is>
-          <t>00:13:59</t>
-        </is>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>But due to the stress, and because the landscape looked all the same, I didn't realize that the ground was coming until way too late.</t>
-        </is>
-      </c>
-      <c r="B169" t="inlineStr">
-        <is>
-          <t>00:13:59</t>
-        </is>
-      </c>
-      <c r="C169" t="inlineStr">
-        <is>
-          <t>00:14:06</t>
-        </is>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>Luckily, we knew the general location of the Cansat thanks to the onboard footage, and it only took us a mere three to four minutes before it was located.</t>
-        </is>
-      </c>
-      <c r="B170" t="inlineStr">
-        <is>
-          <t>00:14:06</t>
-        </is>
-      </c>
-      <c r="C170" t="inlineStr">
-        <is>
-          <t>00:14:15</t>
-        </is>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" t="inlineStr">
-        <is>
-          <t>Somehow, the Kansai was still completely intact with only slight bending in one of the arms.</t>
-        </is>
-      </c>
-      <c r="B171" t="inlineStr">
-        <is>
-          <t>00:14:28</t>
-        </is>
-      </c>
-      <c r="C171" t="inlineStr">
-        <is>
-          <t>00:14:34</t>
-        </is>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" t="inlineStr">
-        <is>
-          <t>So after getting the arms replaced, the satellite was as good as new.</t>
-        </is>
-      </c>
-      <c r="B172" t="inlineStr">
-        <is>
-          <t>00:14:34</t>
-        </is>
-      </c>
-      <c r="C172" t="inlineStr">
-        <is>
-          <t>00:14:38</t>
-        </is>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" t="inlineStr">
-        <is>
-          <t>We even managed to recover our data thanks to this single G force indicator.</t>
-        </is>
-      </c>
-      <c r="B173" t="inlineStr">
-        <is>
-          <t>00:14:38</t>
-        </is>
-      </c>
-      <c r="C173" t="inlineStr">
-        <is>
-          <t>00:14:43</t>
-        </is>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" t="inlineStr">
-        <is>
-          <t>Just make a program to grab the value from every frame, graph it over time, and do some integration.</t>
-        </is>
-      </c>
-      <c r="B174" t="inlineStr">
-        <is>
-          <t>00:14:43</t>
-        </is>
-      </c>
-      <c r="C174" t="inlineStr">
-        <is>
-          <t>00:14:48</t>
-        </is>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" t="inlineStr">
-        <is>
-          <t>And now you have altitude.</t>
-        </is>
-      </c>
-      <c r="B175" t="inlineStr">
-        <is>
-          <t>00:14:48</t>
-        </is>
-      </c>
-      <c r="C175" t="inlineStr">
-        <is>
-          <t>00:14:50</t>
-        </is>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" t="inlineStr">
-        <is>
-          <t>We spent the rest of the day just flying this thing around randomly for fun.</t>
-        </is>
-      </c>
-      <c r="B176" t="inlineStr">
-        <is>
-          <t>00:14:50</t>
-        </is>
-      </c>
-      <c r="C176" t="inlineStr">
-        <is>
-          <t>00:14:54</t>
-        </is>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" t="inlineStr">
-        <is>
-          <t>And we also did this freefall test, and I think I'm now a much better pilot.</t>
-        </is>
-      </c>
-      <c r="B177" t="inlineStr">
-        <is>
-          <t>00:14:54</t>
-        </is>
-      </c>
-      <c r="C177" t="inlineStr">
-        <is>
-          <t>00:14:59</t>
-        </is>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" t="inlineStr">
-        <is>
-          <t>Speaking of that, we were actually offered a second launch on a bigger and more powerful rocket in Seattle during the summer.</t>
-        </is>
-      </c>
-      <c r="B178" t="inlineStr">
-        <is>
-          <t>00:14:59</t>
-        </is>
-      </c>
-      <c r="C178" t="inlineStr">
-        <is>
-          <t>00:15:05</t>
-        </is>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" t="inlineStr">
-        <is>
-          <t>So make sure to let me know in the comments if you are interested.</t>
-        </is>
-      </c>
-      <c r="B179" t="inlineStr">
-        <is>
-          <t>00:15:05</t>
-        </is>
-      </c>
-      <c r="C179" t="inlineStr">
-        <is>
-          <t>00:15:09</t>
-        </is>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" t="inlineStr">
-        <is>
-          <t>And with that being said, special thanks to Zach, Daniel, Emre, Eric and Cynthia for working on this project with me.</t>
-        </is>
-      </c>
-      <c r="B180" t="inlineStr">
-        <is>
-          <t>00:15:13</t>
-        </is>
-      </c>
-      <c r="C180" t="inlineStr">
-        <is>
-          <t>00:15:19</t>
-        </is>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" t="inlineStr">
-        <is>
-          <t>Special thanks to everyone at Kansat who made this experience possible.</t>
-        </is>
-      </c>
-      <c r="B181" t="inlineStr">
-        <is>
-          <t>00:15:19</t>
-        </is>
-      </c>
-      <c r="C181" t="inlineStr">
-        <is>
-          <t>00:15:23</t>
-        </is>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" t="inlineStr">
-        <is>
-          <t>And thank you to you for watching.</t>
-        </is>
-      </c>
-      <c r="B182" t="inlineStr">
-        <is>
-          <t>00:15:23</t>
-        </is>
-      </c>
-      <c r="C182" t="inlineStr">
-        <is>
-          <t>00:15:25</t>
-        </is>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" t="inlineStr">
-        <is>
-          <t>See you next time.</t>
-        </is>
-      </c>
-      <c r="B183" t="inlineStr">
-        <is>
-          <t>00:15:25</t>
-        </is>
-      </c>
-      <c r="C183" t="inlineStr">
-        <is>
-          <t>00:15:27</t>
+          <t>00:15:26</t>
         </is>
       </c>
     </row>

</xml_diff>